<commit_message>
fix bug in 1
</commit_message>
<xml_diff>
--- a/solver/excel/extract/1/高钾归一化.xlsx
+++ b/solver/excel/extract/1/高钾归一化.xlsx
@@ -5,22 +5,33 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\文档\tencent files\527212878\filerecv\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\mathematical_modeling\CUMCM2022\solver\excel\extract\1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59C005D1-EC2A-41CC-AFCE-DFB559D90CA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E835B32-D976-415E-B068-726AEAA966E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="风化" sheetId="1" r:id="rId1"/>
+    <sheet name="无风化" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="71">
   <si>
     <t>二氧化硅(SiO2)_归一化</t>
   </si>
@@ -137,13 +148,621 @@
   </si>
   <si>
     <t>风化</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>高钾</t>
+  </si>
+  <si>
+    <t>无风化</t>
+  </si>
+  <si>
+    <t>03部位1</t>
+  </si>
+  <si>
+    <t>03部位2</t>
+  </si>
+  <si>
+    <t>04</t>
+  </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>06部位1</t>
+  </si>
+  <si>
+    <t>06部位2</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>二氧化硅</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(SiO</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>氧化钠</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(Na</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>O)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>氧化钾</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(K</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>O)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>氧化钙</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(CaO)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>氧化镁</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(MgO)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>氧化铝</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(Al</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>O</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>氧化铁</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(Fe</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>O</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>氧化铜</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(CuO)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>氧化铅</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(PbO)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>氧化钡</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(BaO)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>五氧化二磷</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(P</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>O</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>5</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>氧化锶</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(SrO)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>氧化锡</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(SnO</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>二氧化硫</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(SO</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>纹饰</t>
+  </si>
+  <si>
+    <t>颜色</t>
+  </si>
+  <si>
+    <t>类型</t>
+  </si>
+  <si>
+    <t>总和</t>
+  </si>
+  <si>
+    <t>label</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -165,6 +784,46 @@
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFC00000"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFC00000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFC00000"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <vertAlign val="subscript"/>
+      <sz val="10"/>
+      <color rgb="FFC00000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -202,10 +861,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -547,8 +1222,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AH17" sqref="AH17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -1243,4 +1918,847 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B0D4F7C-E95B-4255-95E7-278A43ECC1A9}">
+  <dimension ref="A1:V12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M33" sqref="M33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:22" ht="27.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="V1" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2">
+        <v>69.33</v>
+      </c>
+      <c r="C2">
+        <v>0.69309264991721298</v>
+      </c>
+      <c r="D2">
+        <v>9.99</v>
+      </c>
+      <c r="E2">
+        <v>6.32</v>
+      </c>
+      <c r="F2">
+        <v>0.87</v>
+      </c>
+      <c r="G2">
+        <v>3.93</v>
+      </c>
+      <c r="H2">
+        <v>1.74</v>
+      </c>
+      <c r="I2">
+        <v>3.87</v>
+      </c>
+      <c r="J2">
+        <v>0.32506658987833797</v>
+      </c>
+      <c r="K2">
+        <v>0.829529911453459</v>
+      </c>
+      <c r="L2">
+        <v>1.17</v>
+      </c>
+      <c r="M2">
+        <v>1.8753149521272799E-2</v>
+      </c>
+      <c r="N2">
+        <v>0.133557699229717</v>
+      </c>
+      <c r="O2">
+        <v>0.39</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2" t="s">
+        <v>40</v>
+      </c>
+      <c r="T2" t="s">
+        <v>41</v>
+      </c>
+      <c r="U2" s="3">
+        <f>SUM(B2:O2)</f>
+        <v>99.61</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3">
+        <v>87.05</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>5.19</v>
+      </c>
+      <c r="E3">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0.78</v>
+      </c>
+      <c r="J3">
+        <v>0.25</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0.66</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <v>2</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="S3" t="s">
+        <v>40</v>
+      </c>
+      <c r="T3" t="s">
+        <v>41</v>
+      </c>
+      <c r="U3" s="3">
+        <f>SUM(B3:O3)</f>
+        <v>100</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4">
+        <v>61.71</v>
+      </c>
+      <c r="C4">
+        <v>0.86273441592457201</v>
+      </c>
+      <c r="D4">
+        <v>12.37</v>
+      </c>
+      <c r="E4">
+        <v>5.87</v>
+      </c>
+      <c r="F4">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="G4">
+        <v>5.5</v>
+      </c>
+      <c r="H4">
+        <v>2.16</v>
+      </c>
+      <c r="I4">
+        <v>5.09</v>
+      </c>
+      <c r="J4">
+        <v>1.41</v>
+      </c>
+      <c r="K4">
+        <v>2.86</v>
+      </c>
+      <c r="L4">
+        <v>0.7</v>
+      </c>
+      <c r="M4">
+        <v>0.1</v>
+      </c>
+      <c r="N4">
+        <v>0.16118305999919499</v>
+      </c>
+      <c r="O4">
+        <v>9.6082524076238296E-2</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="Q4">
+        <v>2</v>
+      </c>
+      <c r="R4">
+        <v>1</v>
+      </c>
+      <c r="S4" t="s">
+        <v>40</v>
+      </c>
+      <c r="T4" t="s">
+        <v>41</v>
+      </c>
+      <c r="U4" s="3">
+        <f>SUM(B4:O4)</f>
+        <v>100</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5">
+        <v>65.88</v>
+      </c>
+      <c r="C5">
+        <v>0.99650935096631399</v>
+      </c>
+      <c r="D5">
+        <v>9.67</v>
+      </c>
+      <c r="E5">
+        <v>7.12</v>
+      </c>
+      <c r="F5">
+        <v>1.56</v>
+      </c>
+      <c r="G5">
+        <v>6.44</v>
+      </c>
+      <c r="H5">
+        <v>2.06</v>
+      </c>
+      <c r="I5">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="J5">
+        <v>0.198087237846581</v>
+      </c>
+      <c r="K5">
+        <v>0.39350682521213498</v>
+      </c>
+      <c r="L5">
+        <v>0.79</v>
+      </c>
+      <c r="M5">
+        <v>2.1823651275647699E-2</v>
+      </c>
+      <c r="N5">
+        <v>0.39007293469932203</v>
+      </c>
+      <c r="O5">
+        <v>0.36</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+      <c r="Q5">
+        <v>2</v>
+      </c>
+      <c r="R5">
+        <v>1</v>
+      </c>
+      <c r="S5" t="s">
+        <v>40</v>
+      </c>
+      <c r="T5" t="s">
+        <v>41</v>
+      </c>
+      <c r="U5" s="3">
+        <f>SUM(B5:O5)</f>
+        <v>98.060000000000016</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6">
+        <v>61.58</v>
+      </c>
+      <c r="C6">
+        <v>0.85162760026377304</v>
+      </c>
+      <c r="D6">
+        <v>10.95</v>
+      </c>
+      <c r="E6">
+        <v>7.35</v>
+      </c>
+      <c r="F6">
+        <v>1.77</v>
+      </c>
+      <c r="G6">
+        <v>7.5</v>
+      </c>
+      <c r="H6">
+        <v>2.62</v>
+      </c>
+      <c r="I6">
+        <v>3.27</v>
+      </c>
+      <c r="J6">
+        <v>0.213704214375637</v>
+      </c>
+      <c r="K6">
+        <v>0.59315388765661503</v>
+      </c>
+      <c r="L6">
+        <v>0.94</v>
+      </c>
+      <c r="M6">
+        <v>0.06</v>
+      </c>
+      <c r="N6">
+        <v>0.34151429770397501</v>
+      </c>
+      <c r="O6">
+        <v>0.47</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
+      <c r="Q6">
+        <v>2</v>
+      </c>
+      <c r="R6">
+        <v>1</v>
+      </c>
+      <c r="S6" t="s">
+        <v>40</v>
+      </c>
+      <c r="T6" t="s">
+        <v>41</v>
+      </c>
+      <c r="U6" s="3">
+        <f>SUM(B6:O6)</f>
+        <v>98.509999999999991</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7">
+        <v>67.650000000000006</v>
+      </c>
+      <c r="C7">
+        <v>0.32627189837106002</v>
+      </c>
+      <c r="D7">
+        <v>7.37</v>
+      </c>
+      <c r="E7">
+        <v>0.55371990574734697</v>
+      </c>
+      <c r="F7">
+        <v>1.98</v>
+      </c>
+      <c r="G7">
+        <v>11.15</v>
+      </c>
+      <c r="H7">
+        <v>2.39</v>
+      </c>
+      <c r="I7">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="J7">
+        <v>0.2</v>
+      </c>
+      <c r="K7">
+        <v>1.38</v>
+      </c>
+      <c r="L7">
+        <v>4.18</v>
+      </c>
+      <c r="M7">
+        <v>0.11</v>
+      </c>
+      <c r="N7">
+        <v>0.11635180821636799</v>
+      </c>
+      <c r="O7">
+        <v>8.36563876651958E-2</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <v>2</v>
+      </c>
+      <c r="R7">
+        <v>1</v>
+      </c>
+      <c r="S7" t="s">
+        <v>40</v>
+      </c>
+      <c r="T7" t="s">
+        <v>41</v>
+      </c>
+      <c r="U7" s="3">
+        <f>SUM(B7:O7)</f>
+        <v>99.999999999999986</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8">
+        <v>59.81</v>
+      </c>
+      <c r="C8">
+        <v>0.70127237510017704</v>
+      </c>
+      <c r="D8">
+        <v>7.68</v>
+      </c>
+      <c r="E8">
+        <v>5.41</v>
+      </c>
+      <c r="F8">
+        <v>1.73</v>
+      </c>
+      <c r="G8">
+        <v>10.050000000000001</v>
+      </c>
+      <c r="H8">
+        <v>6.04</v>
+      </c>
+      <c r="I8">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="J8">
+        <v>0.35</v>
+      </c>
+      <c r="K8">
+        <v>0.97</v>
+      </c>
+      <c r="L8">
+        <v>4.5</v>
+      </c>
+      <c r="M8">
+        <v>0.12</v>
+      </c>
+      <c r="N8">
+        <v>0.252074539139724</v>
+      </c>
+      <c r="O8">
+        <v>0.20665308576008201</v>
+      </c>
+      <c r="P8">
+        <v>1</v>
+      </c>
+      <c r="Q8">
+        <v>2</v>
+      </c>
+      <c r="R8">
+        <v>1</v>
+      </c>
+      <c r="S8" t="s">
+        <v>40</v>
+      </c>
+      <c r="T8" t="s">
+        <v>41</v>
+      </c>
+      <c r="U8" s="3">
+        <f>SUM(B8:O8)</f>
+        <v>99.999999999999986</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9">
+        <v>59.01</v>
+      </c>
+      <c r="C9">
+        <v>2.86</v>
+      </c>
+      <c r="D9">
+        <v>12.53</v>
+      </c>
+      <c r="E9">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="F9">
+        <v>0.207771407912407</v>
+      </c>
+      <c r="G9">
+        <v>6.16</v>
+      </c>
+      <c r="H9">
+        <v>2.88</v>
+      </c>
+      <c r="I9">
+        <v>4.7300000000000004</v>
+      </c>
+      <c r="J9">
+        <v>0.39388028096271299</v>
+      </c>
+      <c r="K9">
+        <v>0.96824966429088699</v>
+      </c>
+      <c r="L9">
+        <v>1.27</v>
+      </c>
+      <c r="M9">
+        <v>1.9340977171779902E-2</v>
+      </c>
+      <c r="N9">
+        <v>0.16446234893089701</v>
+      </c>
+      <c r="O9">
+        <v>0.10629532073133</v>
+      </c>
+      <c r="P9">
+        <v>1</v>
+      </c>
+      <c r="Q9">
+        <v>1</v>
+      </c>
+      <c r="R9">
+        <v>2</v>
+      </c>
+      <c r="S9" t="s">
+        <v>40</v>
+      </c>
+      <c r="T9" t="s">
+        <v>41</v>
+      </c>
+      <c r="U9" s="3">
+        <f>SUM(B9:O9)</f>
+        <v>100</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10">
+        <v>62.47</v>
+      </c>
+      <c r="C10">
+        <v>3.38</v>
+      </c>
+      <c r="D10">
+        <v>12.28</v>
+      </c>
+      <c r="E10">
+        <v>8.23</v>
+      </c>
+      <c r="F10">
+        <v>0.66</v>
+      </c>
+      <c r="G10">
+        <v>9.23</v>
+      </c>
+      <c r="H10">
+        <v>0.5</v>
+      </c>
+      <c r="I10">
+        <v>0.47</v>
+      </c>
+      <c r="J10">
+        <v>1.62</v>
+      </c>
+      <c r="K10">
+        <v>0.28396499840523598</v>
+      </c>
+      <c r="L10">
+        <v>0.16</v>
+      </c>
+      <c r="M10">
+        <v>2.01494917557654E-2</v>
+      </c>
+      <c r="N10">
+        <v>7.0710432527630998E-2</v>
+      </c>
+      <c r="O10">
+        <v>0.62517507731136701</v>
+      </c>
+      <c r="P10">
+        <v>1</v>
+      </c>
+      <c r="Q10">
+        <v>1</v>
+      </c>
+      <c r="R10">
+        <v>4</v>
+      </c>
+      <c r="S10" t="s">
+        <v>40</v>
+      </c>
+      <c r="T10" t="s">
+        <v>41</v>
+      </c>
+      <c r="U10" s="3">
+        <f>SUM(B10:O10)</f>
+        <v>100</v>
+      </c>
+      <c r="V10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11">
+        <v>65.180000000000007</v>
+      </c>
+      <c r="C11">
+        <v>2.1</v>
+      </c>
+      <c r="D11">
+        <v>14.52</v>
+      </c>
+      <c r="E11">
+        <v>8.27</v>
+      </c>
+      <c r="F11">
+        <v>0.52</v>
+      </c>
+      <c r="G11">
+        <v>6.18</v>
+      </c>
+      <c r="H11">
+        <v>0.42</v>
+      </c>
+      <c r="I11">
+        <v>1.07</v>
+      </c>
+      <c r="J11">
+        <v>0.11</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0.22963922433231701</v>
+      </c>
+      <c r="M11">
+        <v>0.04</v>
+      </c>
+      <c r="N11">
+        <v>0.163804178984819</v>
+      </c>
+      <c r="O11">
+        <v>1.1965565966828799</v>
+      </c>
+      <c r="P11">
+        <v>1</v>
+      </c>
+      <c r="Q11">
+        <v>1</v>
+      </c>
+      <c r="R11" s="4">
+        <v>2</v>
+      </c>
+      <c r="S11" t="s">
+        <v>40</v>
+      </c>
+      <c r="T11" t="s">
+        <v>41</v>
+      </c>
+      <c r="U11" s="3">
+        <f>SUM(B11:O11)</f>
+        <v>100</v>
+      </c>
+      <c r="V11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12">
+        <v>79.459999999999994</v>
+      </c>
+      <c r="C12">
+        <v>0.20595188210086901</v>
+      </c>
+      <c r="D12">
+        <v>9.42</v>
+      </c>
+      <c r="E12">
+        <v>0.136700373969213</v>
+      </c>
+      <c r="F12">
+        <v>1.53</v>
+      </c>
+      <c r="G12">
+        <v>3.05</v>
+      </c>
+      <c r="H12">
+        <v>0.175583684505973</v>
+      </c>
+      <c r="I12">
+        <v>9.1096686458835702E-2</v>
+      </c>
+      <c r="J12">
+        <v>0.90884006293435404</v>
+      </c>
+      <c r="K12">
+        <v>0.37499703512780602</v>
+      </c>
+      <c r="L12">
+        <v>1.36</v>
+      </c>
+      <c r="M12">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="N12">
+        <v>2.36</v>
+      </c>
+      <c r="O12">
+        <v>0.10683027490295</v>
+      </c>
+      <c r="P12">
+        <v>1</v>
+      </c>
+      <c r="Q12">
+        <v>2</v>
+      </c>
+      <c r="R12">
+        <v>5</v>
+      </c>
+      <c r="S12" t="s">
+        <v>40</v>
+      </c>
+      <c r="T12" t="s">
+        <v>41</v>
+      </c>
+      <c r="U12" s="3">
+        <f>SUM(B12:O12)</f>
+        <v>99.249999999999986</v>
+      </c>
+      <c r="V12">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>